<commit_message>
rebuild project with 'make all'
</commit_message>
<xml_diff>
--- a/project/excel/bdfkb_schema.xlsx
+++ b/project/excel/bdfkb_schema.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tool" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="ToolCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tool" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,71 +461,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>developer_team</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>technical_area</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>keywords</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
           <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ASKEM_NEU,ASKEM_MIT,ASKEM_NYU,ASKEM_Jataware,Netrias,N3C,BDC,CRA,DNAHIVE,HMS,Stanford,UAB,ICF,SageBio,Insilicom"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"TA1,TA2,TA3"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>entries</t>
         </is>
       </c>
     </row>

</xml_diff>